<commit_message>
Re-organized files and directories
</commit_message>
<xml_diff>
--- a/data/raw_data/field_expt_soil_orgs.xlsx
+++ b/data/raw_data/field_expt_soil_orgs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keithpost/Documents/R files/Ecology Research/grasshopper_soil_animal/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA141A-F399-064B-A58E-98C39382FE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FAF98F-BE54-6243-B14B-30956170BB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12220" yWindow="-24680" windowWidth="21600" windowHeight="19740" tabRatio="659" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12220" yWindow="-24680" windowWidth="27060" windowHeight="19740" tabRatio="659" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Soil-Initial" sheetId="1" r:id="rId1"/>
@@ -28,51 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Plot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil can </t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>extraction (g)</t>
-  </si>
-  <si>
-    <t>Soil for microbial</t>
-  </si>
-  <si>
-    <t>Soil for nematode</t>
-  </si>
-  <si>
-    <t>Soil can + lid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty can </t>
-  </si>
-  <si>
-    <t>+ lid (g)</t>
-  </si>
-  <si>
-    <t>Soil for moisture</t>
-  </si>
-  <si>
-    <t>determination (g)</t>
-  </si>
-  <si>
-    <t>+ dried soil (g)</t>
-  </si>
-  <si>
-    <t>Mite sample</t>
-  </si>
-  <si>
-    <t>soil + bag (g)</t>
-  </si>
-  <si>
-    <t>bag only (g)</t>
   </si>
   <si>
     <t>BF</t>
@@ -112,6 +70,30 @@
   </si>
   <si>
     <t># FF Picked</t>
+  </si>
+  <si>
+    <t>Soil for nematode extraction (g)</t>
+  </si>
+  <si>
+    <t>Soil for microbial extraction (g)</t>
+  </si>
+  <si>
+    <t>Empty can  + lid (g)</t>
+  </si>
+  <si>
+    <t>Soil for moisture determination (g)</t>
+  </si>
+  <si>
+    <t>Soil can + lid + dried soil (g)</t>
+  </si>
+  <si>
+    <t>Mite sample soil + bag (g)</t>
+  </si>
+  <si>
+    <t>Mite sample bag only (g)</t>
+  </si>
+  <si>
+    <t>Soil can  #</t>
   </si>
 </sst>
 </file>
@@ -682,427 +664,402 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="29" style="7" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>201</v>
+      </c>
+      <c r="C3">
+        <v>5.05</v>
+      </c>
+      <c r="D3" s="7">
+        <v>50.39</v>
+      </c>
+      <c r="E3">
+        <v>46.54</v>
+      </c>
+      <c r="F3">
+        <v>50.3</v>
+      </c>
+      <c r="G3">
+        <v>94.83</v>
+      </c>
+      <c r="H3">
+        <v>357.39</v>
+      </c>
+      <c r="I3">
+        <v>12.07</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="C4">
-        <v>5.05</v>
+        <v>5.07</v>
       </c>
       <c r="D4" s="7">
-        <v>50.39</v>
+        <v>50.01</v>
       </c>
       <c r="E4">
-        <v>46.54</v>
+        <v>45.74</v>
       </c>
       <c r="F4">
-        <v>50.3</v>
+        <v>50.46</v>
       </c>
       <c r="G4">
-        <v>94.83</v>
+        <v>93.686999999999998</v>
       </c>
       <c r="H4">
-        <v>357.39</v>
+        <v>193.89</v>
       </c>
       <c r="I4">
-        <v>12.07</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>221</v>
+        <v>117</v>
       </c>
       <c r="C5">
-        <v>5.07</v>
+        <v>4.96</v>
       </c>
       <c r="D5" s="7">
-        <v>50.01</v>
+        <v>50.75</v>
       </c>
       <c r="E5">
-        <v>45.74</v>
+        <v>46.69</v>
       </c>
       <c r="F5">
-        <v>50.46</v>
+        <v>50.65</v>
       </c>
       <c r="G5">
-        <v>93.686999999999998</v>
+        <v>94.563000000000002</v>
       </c>
       <c r="H5">
-        <v>193.89</v>
+        <v>223.4</v>
       </c>
       <c r="I5">
-        <v>11.99</v>
+        <v>11.98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="C6">
-        <v>4.96</v>
+        <v>5.01</v>
       </c>
       <c r="D6" s="7">
-        <v>50.75</v>
+        <v>50.18</v>
       </c>
       <c r="E6">
-        <v>46.69</v>
+        <v>46.16</v>
       </c>
       <c r="F6">
-        <v>50.65</v>
+        <v>49.69</v>
       </c>
       <c r="G6">
-        <v>94.563000000000002</v>
+        <v>94.009</v>
       </c>
       <c r="H6">
-        <v>223.4</v>
+        <v>334.58</v>
       </c>
       <c r="I6">
-        <v>11.98</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="C7">
-        <v>5.01</v>
+        <v>4.99</v>
       </c>
       <c r="D7" s="7">
-        <v>50.18</v>
+        <v>50.07</v>
       </c>
       <c r="E7">
-        <v>46.16</v>
+        <v>46.04</v>
       </c>
       <c r="F7">
-        <v>49.69</v>
+        <v>50.62</v>
       </c>
       <c r="G7">
-        <v>94.009</v>
+        <v>94.477999999999994</v>
       </c>
       <c r="H7">
-        <v>334.58</v>
+        <v>284.11</v>
       </c>
       <c r="I7">
-        <v>11.67</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>207</v>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>4.99</v>
+        <v>5.03</v>
       </c>
       <c r="D8" s="7">
-        <v>50.07</v>
+        <v>49.96</v>
       </c>
       <c r="E8">
-        <v>46.04</v>
+        <v>46.08</v>
       </c>
       <c r="F8">
         <v>50.62</v>
       </c>
       <c r="G8">
-        <v>94.477999999999994</v>
+        <v>94.721000000000004</v>
       </c>
       <c r="H8">
-        <v>284.11</v>
+        <v>383.52</v>
       </c>
       <c r="I8">
-        <v>11.76</v>
+        <v>11.86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>21</v>
-      </c>
       <c r="C9">
-        <v>5.03</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="D9" s="7">
-        <v>49.96</v>
+        <v>50.05</v>
       </c>
       <c r="E9">
-        <v>46.08</v>
+        <v>46.56</v>
       </c>
       <c r="F9">
-        <v>50.62</v>
+        <v>49.98</v>
       </c>
       <c r="G9">
-        <v>94.721000000000004</v>
+        <v>94.149000000000001</v>
       </c>
       <c r="H9">
-        <v>383.52</v>
+        <v>162.13</v>
       </c>
       <c r="I9">
-        <v>11.86</v>
+        <v>11.87</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="C10">
-        <v>5.0199999999999996</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="D10" s="7">
-        <v>50.05</v>
+        <v>50.41</v>
       </c>
       <c r="E10">
-        <v>46.56</v>
+        <v>45.7</v>
       </c>
       <c r="F10">
-        <v>49.98</v>
+        <v>50.03</v>
       </c>
       <c r="G10">
-        <v>94.149000000000001</v>
+        <v>93.456999999999994</v>
       </c>
       <c r="H10">
-        <v>162.13</v>
+        <v>314.04000000000002</v>
       </c>
       <c r="I10">
-        <v>11.87</v>
+        <v>11.94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="C11">
-        <v>4.9800000000000004</v>
+        <v>5.01</v>
       </c>
       <c r="D11" s="7">
-        <v>50.41</v>
+        <v>49.64</v>
       </c>
       <c r="E11">
-        <v>45.7</v>
+        <v>45.99</v>
       </c>
       <c r="F11">
-        <v>50.03</v>
+        <v>49.92</v>
       </c>
       <c r="G11">
-        <v>93.456999999999994</v>
+        <v>94.126000000000005</v>
       </c>
       <c r="H11">
-        <v>314.04000000000002</v>
+        <v>401.94</v>
       </c>
       <c r="I11">
-        <v>11.94</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>213</v>
+        <v>90</v>
       </c>
       <c r="C12">
         <v>5.01</v>
       </c>
       <c r="D12" s="7">
-        <v>49.64</v>
+        <v>50.11</v>
       </c>
       <c r="E12">
-        <v>45.99</v>
+        <v>46.1</v>
       </c>
       <c r="F12">
-        <v>49.92</v>
+        <v>50.79</v>
       </c>
       <c r="G12">
-        <v>94.126000000000005</v>
+        <v>94.745999999999995</v>
       </c>
       <c r="H12">
-        <v>401.94</v>
+        <v>409.22</v>
       </c>
       <c r="I12">
-        <v>11.9</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C13">
-        <v>5.01</v>
+        <v>5.04</v>
       </c>
       <c r="D13" s="7">
-        <v>50.11</v>
+        <v>50.1</v>
       </c>
       <c r="E13">
-        <v>46.1</v>
+        <v>46.19</v>
       </c>
       <c r="F13">
-        <v>50.79</v>
+        <v>50.48</v>
       </c>
       <c r="G13">
-        <v>94.745999999999995</v>
+        <v>94.54</v>
       </c>
       <c r="H13">
-        <v>409.22</v>
+        <v>328.77</v>
       </c>
       <c r="I13">
-        <v>11.99</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>5.04</v>
+        <v>5.05</v>
       </c>
       <c r="D14" s="7">
-        <v>50.1</v>
+        <v>49.78</v>
       </c>
       <c r="E14">
-        <v>46.19</v>
+        <v>46.4</v>
       </c>
       <c r="F14">
-        <v>50.48</v>
+        <v>49.94</v>
       </c>
       <c r="G14">
-        <v>94.54</v>
+        <v>94.426000000000002</v>
       </c>
       <c r="H14">
-        <v>328.77</v>
+        <v>384.19</v>
       </c>
       <c r="I14">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>5.05</v>
-      </c>
-      <c r="D15" s="7">
-        <v>49.78</v>
-      </c>
-      <c r="E15">
-        <v>46.4</v>
-      </c>
-      <c r="F15">
-        <v>49.94</v>
-      </c>
-      <c r="G15">
-        <v>94.426000000000002</v>
-      </c>
-      <c r="H15">
-        <v>384.19</v>
-      </c>
-      <c r="I15">
         <v>11.92</v>
       </c>
     </row>
@@ -1119,428 +1076,402 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>5.07</v>
+      </c>
+      <c r="D3" s="7">
+        <v>50.46</v>
+      </c>
+      <c r="E3">
+        <v>45.85</v>
+      </c>
+      <c r="F3">
+        <v>50.25</v>
+      </c>
+      <c r="G3">
+        <v>92.185000000000002</v>
+      </c>
+      <c r="H3">
+        <v>361.92</v>
+      </c>
+      <c r="I3">
+        <v>13.15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C4">
-        <v>5.07</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="D4" s="7">
-        <v>50.46</v>
+        <v>50.2</v>
       </c>
       <c r="E4">
-        <v>45.85</v>
+        <v>46.15</v>
       </c>
       <c r="F4">
-        <v>50.25</v>
+        <v>50.54</v>
       </c>
       <c r="G4">
-        <v>92.185000000000002</v>
+        <v>91.866</v>
       </c>
       <c r="H4">
-        <v>361.92</v>
+        <v>404.46</v>
       </c>
       <c r="I4">
-        <v>13.15</v>
+        <v>13.23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="C5">
-        <v>4.8899999999999997</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="D5" s="7">
-        <v>50.2</v>
+        <v>50.65</v>
       </c>
       <c r="E5">
-        <v>46.15</v>
+        <v>45.93</v>
       </c>
       <c r="F5">
-        <v>50.54</v>
+        <v>50.1</v>
       </c>
       <c r="G5">
-        <v>91.866</v>
+        <v>90.728999999999999</v>
       </c>
       <c r="H5">
-        <v>404.46</v>
+        <v>365.85</v>
       </c>
       <c r="I5">
-        <v>13.23</v>
+        <v>12.81</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="C6">
-        <v>4.9400000000000004</v>
+        <v>4.95</v>
       </c>
       <c r="D6" s="7">
-        <v>50.65</v>
+        <v>50.22</v>
       </c>
       <c r="E6">
-        <v>45.93</v>
+        <v>46.2</v>
       </c>
       <c r="F6">
-        <v>50.1</v>
+        <v>50.06</v>
       </c>
       <c r="G6">
-        <v>90.728999999999999</v>
+        <v>92.352000000000004</v>
       </c>
       <c r="H6">
-        <v>365.85</v>
+        <v>413.11</v>
       </c>
       <c r="I6">
-        <v>12.81</v>
+        <v>11.83</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>169</v>
+        <v>91</v>
       </c>
       <c r="C7">
-        <v>4.95</v>
+        <v>5</v>
       </c>
       <c r="D7" s="7">
-        <v>50.22</v>
+        <v>50.16</v>
       </c>
       <c r="E7">
-        <v>46.2</v>
+        <v>46.22</v>
       </c>
       <c r="F7">
-        <v>50.06</v>
+        <v>50.3</v>
       </c>
       <c r="G7">
-        <v>92.352000000000004</v>
+        <v>92.308000000000007</v>
       </c>
       <c r="H7">
-        <v>413.11</v>
+        <v>375.52</v>
       </c>
       <c r="I7">
-        <v>11.83</v>
+        <v>12.92</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>5.07</v>
       </c>
       <c r="D8" s="7">
-        <v>50.16</v>
+        <v>50.24</v>
       </c>
       <c r="E8">
-        <v>46.22</v>
+        <v>45.91</v>
       </c>
       <c r="F8">
-        <v>50.3</v>
+        <v>50.58</v>
       </c>
       <c r="G8">
-        <v>92.308000000000007</v>
+        <v>92.634</v>
       </c>
       <c r="H8">
-        <v>375.52</v>
+        <v>443.6</v>
       </c>
       <c r="I8">
-        <v>12.92</v>
+        <v>12.46</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C9">
-        <v>5.07</v>
+        <v>5.05</v>
       </c>
       <c r="D9" s="7">
-        <v>50.24</v>
+        <v>49.91</v>
       </c>
       <c r="E9">
-        <v>45.91</v>
+        <v>45.82</v>
       </c>
       <c r="F9">
-        <v>50.58</v>
+        <v>49.89</v>
       </c>
       <c r="G9">
-        <v>92.634</v>
+        <v>91.873000000000005</v>
       </c>
       <c r="H9">
-        <v>443.6</v>
+        <v>408.18</v>
       </c>
       <c r="I9">
-        <v>12.46</v>
+        <v>12.19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C10">
-        <v>5.05</v>
+        <v>5.04</v>
       </c>
       <c r="D10" s="7">
-        <v>49.91</v>
+        <v>50.34</v>
       </c>
       <c r="E10">
-        <v>45.82</v>
+        <v>45.93</v>
       </c>
       <c r="F10">
-        <v>49.89</v>
+        <v>49.45</v>
       </c>
       <c r="G10">
-        <v>91.873000000000005</v>
+        <v>90.936999999999998</v>
       </c>
       <c r="H10">
-        <v>408.18</v>
+        <v>388.54</v>
       </c>
       <c r="I10">
-        <v>12.19</v>
+        <v>12.23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C11">
-        <v>5.04</v>
+        <v>5.09</v>
       </c>
       <c r="D11" s="7">
-        <v>50.34</v>
+        <v>49.9</v>
       </c>
       <c r="E11">
-        <v>45.93</v>
+        <v>46.05</v>
       </c>
       <c r="F11">
-        <v>49.45</v>
+        <v>49.97</v>
       </c>
       <c r="G11">
-        <v>90.936999999999998</v>
+        <v>92.602000000000004</v>
       </c>
       <c r="H11">
-        <v>388.54</v>
+        <v>464.05</v>
       </c>
       <c r="I11">
-        <v>12.23</v>
+        <v>12.14</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>101</v>
+        <v>206</v>
       </c>
       <c r="C12">
-        <v>5.09</v>
+        <v>4.93</v>
       </c>
       <c r="D12" s="7">
-        <v>49.9</v>
+        <v>50.11</v>
       </c>
       <c r="E12">
-        <v>46.05</v>
+        <v>46.14</v>
       </c>
       <c r="F12">
-        <v>49.97</v>
+        <v>49.75</v>
       </c>
       <c r="G12">
-        <v>92.602000000000004</v>
+        <v>91.867999999999995</v>
       </c>
       <c r="H12">
-        <v>464.05</v>
+        <v>373.27</v>
       </c>
       <c r="I12">
-        <v>12.14</v>
+        <v>12.16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>206</v>
+        <v>46</v>
       </c>
       <c r="C13">
-        <v>4.93</v>
+        <v>5.08</v>
       </c>
       <c r="D13" s="7">
-        <v>50.11</v>
+        <v>50.13</v>
       </c>
       <c r="E13">
-        <v>46.14</v>
+        <v>46.28</v>
       </c>
       <c r="F13">
-        <v>49.75</v>
+        <v>49.93</v>
       </c>
       <c r="G13">
-        <v>91.867999999999995</v>
+        <v>92.352000000000004</v>
       </c>
       <c r="H13">
-        <v>373.27</v>
+        <v>386.52</v>
       </c>
       <c r="I13">
-        <v>12.16</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C14">
-        <v>5.08</v>
+        <v>5.05</v>
       </c>
       <c r="D14" s="7">
-        <v>50.13</v>
+        <v>49.88</v>
       </c>
       <c r="E14">
-        <v>46.28</v>
+        <v>45.75</v>
       </c>
       <c r="F14">
-        <v>49.93</v>
+        <v>50.17</v>
       </c>
       <c r="G14">
-        <v>92.352000000000004</v>
+        <v>92.405000000000001</v>
       </c>
       <c r="H14">
-        <v>386.52</v>
+        <v>398.43</v>
       </c>
       <c r="I14">
-        <v>11.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>56</v>
-      </c>
-      <c r="C15">
-        <v>5.05</v>
-      </c>
-      <c r="D15" s="7">
-        <v>49.88</v>
-      </c>
-      <c r="E15">
-        <v>45.75</v>
-      </c>
-      <c r="F15">
-        <v>50.17</v>
-      </c>
-      <c r="G15">
-        <v>92.405000000000001</v>
-      </c>
-      <c r="H15">
-        <v>398.43</v>
-      </c>
-      <c r="I15">
         <v>11.97</v>
       </c>
     </row>
@@ -1567,12 +1498,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1580,25 +1511,25 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1915,12 +1846,12 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1930,25 +1861,25 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2332,12 +2263,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2345,22 +2276,22 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2653,12 +2584,12 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -2666,22 +2597,22 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>